<commit_message>
Updated programs.py to read excel data
</commit_message>
<xml_diff>
--- a/assets/Files/Sector_DevOps_Status_FX.xlsx
+++ b/assets/Files/Sector_DevOps_Status_FX.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stephen.french\Desktop\dsc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\Repos\DevOps\resources\assets\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,9 +35,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="40">
   <si>
-    <t>Row Labels</t>
-  </si>
-  <si>
     <t>DevOps Status</t>
   </si>
   <si>
@@ -80,9 +77,6 @@
     <t>% programs doing DevOps</t>
   </si>
   <si>
-    <t>Average Head count</t>
-  </si>
-  <si>
     <t>Tool Notes</t>
   </si>
   <si>
@@ -153,6 +147,12 @@
   </si>
   <si>
     <t>Using XAML builds</t>
+  </si>
+  <si>
+    <t>Average Head Count</t>
+  </si>
+  <si>
+    <t>Program Name</t>
   </si>
 </sst>
 </file>
@@ -199,21 +199,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -293,38 +278,123 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="18">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -352,6 +422,20 @@
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -364,6 +448,27 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J17" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="17" tableBorderDxfId="16">
+  <autoFilter ref="A1:J17"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="Program Name" dataDxfId="11"/>
+    <tableColumn id="2" name="Average Head Count" dataDxfId="10"/>
+    <tableColumn id="3" name="Chief Software Engineer" dataDxfId="9"/>
+    <tableColumn id="4" name="DevOps Status" dataDxfId="8">
+      <calculatedColumnFormula>IF((AND(F2="Yes",G2="Yes",H2="Yes")),"Continue",IF((OR(F2="Yes",G2="Yes",H2="Yes")),"Planned",IF((AND(F2="No",G2="No",H2="No")),"No")))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="Infrastructure" dataDxfId="7"/>
+    <tableColumn id="6" name="Build Pipeline" dataDxfId="6"/>
+    <tableColumn id="7" name="Continuous Integration" dataDxfId="5"/>
+    <tableColumn id="8" name="Continuous Deployment" dataDxfId="4"/>
+    <tableColumn id="9" name="Notes" dataDxfId="3"/>
+    <tableColumn id="10" name="Tool Notes" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -667,478 +772,543 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="58.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" customWidth="1"/>
+    <col min="9" max="9" width="58.7109375" style="2" customWidth="1"/>
     <col min="10" max="10" width="58.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="E1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="str">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15" t="str">
         <f t="shared" ref="D2:D7" si="0">IF((AND(F2="Yes",G2="Yes",H2="Yes")),"Continue",IF((OR(F2="Yes",G2="Yes",H2="Yes")),"Planned",IF((AND(F2="No",G2="No",H2="No")),"No")))</f>
         <v>Continue</v>
       </c>
-      <c r="F2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" t="s">
-        <v>37</v>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="16"/>
+      <c r="J2" s="15" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="str">
+      <c r="A3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15" t="str">
         <f t="shared" si="0"/>
         <v>Planned</v>
       </c>
-      <c r="F3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" t="s">
-        <v>36</v>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="16"/>
+      <c r="J3" s="15" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="str">
+      <c r="A4" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15" t="str">
         <f t="shared" si="0"/>
         <v>Planned</v>
       </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" t="s">
-        <v>36</v>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="16"/>
+      <c r="J4" s="15" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="str">
+      <c r="A5" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15" t="str">
         <f t="shared" si="0"/>
         <v>Continue</v>
       </c>
-      <c r="F5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" t="s">
-        <v>37</v>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="16"/>
+      <c r="J5" s="15" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="str">
+      <c r="A6" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15" t="str">
         <f t="shared" si="0"/>
         <v>Continue</v>
       </c>
-      <c r="F6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" t="s">
-        <v>37</v>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="16"/>
+      <c r="J6" s="15" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" t="str">
+      <c r="A7" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15" t="str">
         <f t="shared" si="0"/>
         <v>Continue</v>
       </c>
-      <c r="F7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" t="s">
-        <v>37</v>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="16"/>
+      <c r="J7" s="15" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="str">
+      <c r="A8" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15" t="str">
         <f>IF((AND(F8="Yes",G8="Yes",H8="Yes")),"Continue",IF((OR(F8="Yes",G8="Yes",H8="Yes")),"Planned",IF((AND(F8="No",G8="No",H8="No")),"No")))</f>
         <v>Planned</v>
       </c>
-      <c r="F8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" t="s">
-        <v>39</v>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="16"/>
+      <c r="J8" s="15" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" t="str">
+      <c r="A9" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15" t="str">
         <f t="shared" ref="D9:D17" si="1">IF((AND(F9="Yes",G9="Yes",H9="Yes")),"Continue",IF((OR(F9="Yes",G9="Yes",H9="Yes")),"Planned",IF((AND(F9="No",G9="No",H9="No")),"No")))</f>
         <v>Planned</v>
       </c>
-      <c r="F9" t="s">
+      <c r="E9" s="15"/>
+      <c r="F9" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="16"/>
+      <c r="J9" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" t="str">
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15" t="str">
         <f t="shared" si="1"/>
         <v>Planned</v>
       </c>
-      <c r="F10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="E10" s="15"/>
+      <c r="F10" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="16"/>
+      <c r="J10" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="J10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" t="str">
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15" t="str">
         <f t="shared" si="1"/>
         <v>Planned</v>
       </c>
-      <c r="F11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" t="s">
-        <v>25</v>
-      </c>
-      <c r="J11" t="s">
-        <v>37</v>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="16"/>
+      <c r="J11" s="15" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" t="str">
+      <c r="A12" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15" t="str">
         <f t="shared" si="1"/>
         <v>Planned</v>
       </c>
-      <c r="F12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" t="s">
-        <v>25</v>
-      </c>
-      <c r="J12" t="s">
-        <v>37</v>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="16"/>
+      <c r="J12" s="15" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" t="str">
+      <c r="A13" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15" t="str">
         <f t="shared" si="1"/>
         <v>No</v>
       </c>
-      <c r="F13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" t="s">
-        <v>25</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J13" t="s">
-        <v>38</v>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" t="str">
+      <c r="A14" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15" t="str">
         <f t="shared" si="1"/>
         <v>Planned</v>
       </c>
-      <c r="F14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G14" t="s">
-        <v>24</v>
-      </c>
-      <c r="H14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J14" t="s">
-        <v>37</v>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="16"/>
+      <c r="J14" s="15" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" t="str">
+      <c r="A15" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15" t="str">
         <f t="shared" si="1"/>
         <v>Planned</v>
       </c>
-      <c r="F15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" t="s">
-        <v>24</v>
-      </c>
-      <c r="H15" t="s">
-        <v>25</v>
-      </c>
-      <c r="J15" t="s">
-        <v>37</v>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="16"/>
+      <c r="J15" s="15" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" t="str">
+      <c r="A16" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15" t="str">
         <f t="shared" si="1"/>
         <v>Planned</v>
       </c>
-      <c r="F16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" t="s">
-        <v>24</v>
-      </c>
-      <c r="H16" t="s">
-        <v>25</v>
-      </c>
-      <c r="J16" t="s">
-        <v>37</v>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="16"/>
+      <c r="J16" s="15" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" t="str">
+      <c r="A17" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15" t="str">
         <f t="shared" si="1"/>
         <v>Continue</v>
       </c>
-      <c r="F17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17" t="s">
-        <v>24</v>
-      </c>
-      <c r="H17" t="s">
-        <v>24</v>
-      </c>
-      <c r="J17" t="s">
-        <v>37</v>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="16"/>
+      <c r="J17" s="15" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C27" s="6" t="s">
+      <c r="A27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="8">
+      <c r="C27" s="5">
         <f>SUM(B2:B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C28" s="9"/>
-      <c r="D28" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="11" t="e">
+      <c r="A28" s="6"/>
+      <c r="B28" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="8" t="e">
         <f>SUM(SUMIFS(#REF!,#REF!, {"Planned","Continue"}))</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C29" s="9"/>
-      <c r="D29" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="12" t="e">
-        <f>E28/E27</f>
+      <c r="A29" s="6"/>
+      <c r="B29" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="9" t="e">
+        <f>C28/C27</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C30" s="9"/>
-      <c r="D30" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="11">
+      <c r="A30" s="6"/>
+      <c r="B30" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="8">
         <f>COUNTA(A2:A17)</f>
         <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C31" s="9"/>
-      <c r="D31" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E31" s="11">
+      <c r="A31" s="6"/>
+      <c r="B31" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="8">
         <f>COUNTIF(D2:D17,"Planned")+COUNTIF(D2:D17,"Continue")</f>
         <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="13"/>
-      <c r="D32" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E32" s="15">
-        <f>E31/E30</f>
+      <c r="A32" s="10"/>
+      <c r="B32" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="12">
+        <f>C31/C30</f>
         <v>0.9375</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1"/>
   <conditionalFormatting sqref="D2:D17">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
       <formula>"Planned"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>"Continue"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:H17 J2:J17">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:H17 J2:J17">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>